<commit_message>
Changing spreadsheet path finding to release
</commit_message>
<xml_diff>
--- a/MATERIAL/Exporter/SpreadsheetToJson.xlsx
+++ b/MATERIAL/Exporter/SpreadsheetToJson.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Academic\waiting-game-DD-software\MATERIAL\SpreadsheetToJson\SpreadsheetToJson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9B9A33-18D7-4C8F-8929-DDFE6EF3CB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C247105-964B-4EE5-BBE1-AB8DD22DEF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="30960" windowHeight="12120" activeTab="6" xr2:uid="{B6D18B84-30F9-47D4-B577-8C2C411769BF}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="30960" windowHeight="12120" xr2:uid="{B6D18B84-30F9-47D4-B577-8C2C411769BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trainings" sheetId="1" r:id="rId1"/>
-    <sheet name="Experiments" sheetId="2" r:id="rId2"/>
+    <sheet name="Practices" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
     <sheet name="Texts" sheetId="3" r:id="rId3"/>
-    <sheet name="Prizes" sheetId="4" r:id="rId4"/>
-    <sheet name="Times" sheetId="5" r:id="rId5"/>
+    <sheet name="Rewards" sheetId="4" r:id="rId4"/>
+    <sheet name="Delays" sheetId="5" r:id="rId5"/>
     <sheet name="Debug" sheetId="6" r:id="rId6"/>
     <sheet name="Export" sheetId="8" r:id="rId7"/>
   </sheets>
@@ -42,18 +42,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="111">
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>Immediate Prize Value</t>
-  </si>
-  <si>
-    <t>Second Prize Lane</t>
-  </si>
-  <si>
-    <t>Second Prize Value</t>
   </si>
   <si>
     <t>Language</t>
@@ -374,13 +365,34 @@
     <t>Value</t>
   </si>
   <si>
-    <t>pista</t>
-  </si>
-  <si>
-    <t>tempo</t>
-  </si>
-  <si>
     <t>Always Imaginary First</t>
+  </si>
+  <si>
+    <t>Restart Game</t>
+  </si>
+  <si>
+    <t>Reiniciar o jogo</t>
+  </si>
+  <si>
+    <t>Restart game</t>
+  </si>
+  <si>
+    <t>Reiniciar el juego</t>
+  </si>
+  <si>
+    <t>Lane</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Immediate Reward Value</t>
+  </si>
+  <si>
+    <t>Delayed Reward Lane</t>
+  </si>
+  <si>
+    <t>Delayed Reward Value</t>
   </si>
 </sst>
 </file>
@@ -562,7 +574,7 @@
                   <a14:compatExt spid="_x0000_s8193"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{657A5E4E-C797-3894-EB03-844117DC360D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000001200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -582,27 +594,16 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
-                  <a:tailEnd type="none" w="med" len="med"/>
+                  <a:tailEnd/>
                 </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -935,8 +936,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,13 +951,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1084,7 +1085,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,13 +1099,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1621,337 +1622,349 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6C1F5F-4C6A-4FD8-A57E-4A83108ED982}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:27" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="X2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="X2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:27" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="X3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="AA3" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="91.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="X3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Z3" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="91.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="X4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="Z4" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="AA4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -1978,6 +1991,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2002,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2050,17 +2064,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2116,7 +2130,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2126,10 +2140,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2137,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2152,7 +2166,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2198,7 +2212,7 @@
 </file>
 
 <file path=vstoDataStore/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08DE89BB-58F4-4E17-841E-C222C37C3F39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E4729BE-7A32-438D-BDB3-F278A4D64197}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>